<commit_message>
heuristic_analysis improved after first review
</commit_message>
<xml_diff>
--- a/heuristic_analysis/planning solutios analysis.xlsx
+++ b/heuristic_analysis/planning solutios analysis.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis non-heuristic" sheetId="3" r:id="rId1"/>
     <sheet name="Analysis heuristic" sheetId="4" r:id="rId2"/>
     <sheet name="Analysis both" sheetId="5" r:id="rId3"/>
+    <sheet name="Plot Problem 1" sheetId="6" r:id="rId4"/>
+    <sheet name="Plot Problem 2" sheetId="7" r:id="rId5"/>
+    <sheet name="Plot Problem 3" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="21">
   <si>
     <t>uniform_cost_search</t>
   </si>
@@ -78,6 +81,12 @@
   </si>
   <si>
     <t>Optimality based on Time Elapsed</t>
+  </si>
+  <si>
+    <t>Optimality Node expansions</t>
+  </si>
+  <si>
+    <t>Optimality Time Elapsed</t>
   </si>
 </sst>
 </file>
@@ -358,6 +367,4232 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Optimality Problem 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10275315453729129"/>
+          <c:y val="0.14462041965424713"/>
+          <c:w val="0.85066028578991892"/>
+          <c:h val="0.70759653367351416"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Plot Problem 1'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimality Node expansions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.7222222222222221E-2"/>
+                  <c:y val="-1.8518518518518517E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>breadth_first</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-5366-4792-BFE4-16B38DA3D0FE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>depth_first_graph</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.22655555555555559"/>
+                      <c:h val="6.4745552639253412E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-5366-4792-BFE4-16B38DA3D0FE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.7220034995625041E-3"/>
+                  <c:y val="5.3240740740740741E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>uniform_cost_search</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.2936111111111111"/>
+                      <c:h val="8.3194444444444446E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-5366-4792-BFE4-16B38DA3D0FE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.05"/>
+                  <c:y val="1.8226888305628463E-7"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0665C7DF-AF98-4E9D-81B4-1359A61B0C82}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLREF]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.26930555555555558"/>
+                      <c:h val="6.4745552639253412E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{0665C7DF-AF98-4E9D-81B4-1359A61B0C82}</c15:txfldGUID>
+                      <c15:f>'Plot Problem 1'!$A$5</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>h_ignore_preconditions</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-5366-4792-BFE4-16B38DA3D0FE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.18888888888888891"/>
+                  <c:y val="-1.8518336249635461E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7FE95BE8-9B83-46AA-A893-CC7CF52AF27D}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLREF]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.18719444444444444"/>
+                      <c:h val="6.4745552639253412E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{7FE95BE8-9B83-46AA-A893-CC7CF52AF27D}</c15:txfldGUID>
+                      <c15:f>'Plot Problem 1'!$A$6</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>h_pg_levelsum</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-5366-4792-BFE4-16B38DA3D0FE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Plot Problem 1'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Plot Problem 1'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>49.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5366-4792-BFE4-16B38DA3D0FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="687801040"/>
+        <c:axId val="687802352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="687801040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="110"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Optimality</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Nr Node Expansions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="687802352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="687802352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Optimality Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Elapsed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="687801040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Optimality Problem 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10275315453729129"/>
+          <c:y val="0.10886622971011307"/>
+          <c:w val="0.85066028578991892"/>
+          <c:h val="0.74335072361764831"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Plot Problem 2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimality Node expansions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.7222222222222221E-2"/>
+                  <c:y val="-1.8518518518518517E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>breadth_first</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-0228-4632-ADA8-DA4BED4C3BFA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.4825313117996042E-2"/>
+                  <c:y val="-3.128491620111748E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>depth_first_graph</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-0228-4632-ADA8-DA4BED4C3BFA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.7220034995625041E-3"/>
+                  <c:y val="5.3240740740740741E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>uniform_cost_search</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.2936111111111111"/>
+                      <c:h val="8.3194444444444446E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-0228-4632-ADA8-DA4BED4C3BFA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.05"/>
+                  <c:y val="1.8226888305628463E-7"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0665C7DF-AF98-4E9D-81B4-1359A61B0C82}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLREF]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.26930555555555558"/>
+                      <c:h val="6.4745552639253412E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{0665C7DF-AF98-4E9D-81B4-1359A61B0C82}</c15:txfldGUID>
+                      <c15:f>'Plot Problem 2'!$A$5</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>h_ignore_preconditions</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-0228-4632-ADA8-DA4BED4C3BFA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.18888888888888891"/>
+                  <c:y val="-1.8518336249635461E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7FE95BE8-9B83-46AA-A893-CC7CF52AF27D}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLREF]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.18719444444444444"/>
+                      <c:h val="6.4745552639253412E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{7FE95BE8-9B83-46AA-A893-CC7CF52AF27D}</c15:txfldGUID>
+                      <c15:f>'Plot Problem 2'!$A$6</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>h_pg_levelsum</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-0228-4632-ADA8-DA4BED4C3BFA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Plot Problem 2'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Plot Problem 2'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>37.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0228-4632-ADA8-DA4BED4C3BFA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="687801040"/>
+        <c:axId val="687802352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="687801040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="110"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Optimality</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Nr Node Expansions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="687802352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="687802352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Optimality Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Elapsed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="687801040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Optimality Problem 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10275315453729129"/>
+          <c:y val="0.13568187216821362"/>
+          <c:w val="0.85066028578991892"/>
+          <c:h val="0.71653508115954767"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Plot Problem 3'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimality Node expansions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.7222222222222221E-2"/>
+                  <c:y val="-1.8518518518518517E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>breadth_first</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-AB7D-4344-9D21-A2AF81A6AA5C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>depth_first_graph</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-AB7D-4344-9D21-A2AF81A6AA5C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.7220034995625041E-3"/>
+                  <c:y val="5.3240740740740741E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>uniform_cost_search</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.2936111111111111"/>
+                      <c:h val="8.3194444444444446E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-AB7D-4344-9D21-A2AF81A6AA5C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.05"/>
+                  <c:y val="1.8226888305628463E-7"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0665C7DF-AF98-4E9D-81B4-1359A61B0C82}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLREF]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.26930555555555558"/>
+                      <c:h val="6.4745552639253412E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{0665C7DF-AF98-4E9D-81B4-1359A61B0C82}</c15:txfldGUID>
+                      <c15:f>'Plot Problem 3'!$A$5</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>h_ignore_preconditions</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-AB7D-4344-9D21-A2AF81A6AA5C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.18888888888888891"/>
+                  <c:y val="-1.8518336249635461E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7FE95BE8-9B83-46AA-A893-CC7CF52AF27D}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLREF]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.18719444444444444"/>
+                      <c:h val="6.4745552639253412E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{7FE95BE8-9B83-46AA-A893-CC7CF52AF27D}</c15:txfldGUID>
+                      <c15:f>'Plot Problem 3'!$A$6</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>h_pg_levelsum</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-AB7D-4344-9D21-A2AF81A6AA5C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Plot Problem 3'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Plot Problem 3'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-AB7D-4344-9D21-A2AF81A6AA5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="687801040"/>
+        <c:axId val="687802352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="687801040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="110"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Optimality</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Nr Node Expansions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="687802352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="687802352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Optimality Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Elapsed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="687801040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>136524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>454025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>31749</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{932457E6-B6C7-4147-B9F2-47BB77F44770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>136524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>454025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>31749</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97473B62-CABB-4851-9AF4-469634CF9AD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>136524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>454025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>31749</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{579011B6-5672-41A4-B3DB-7D20DD972B4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1313,8 +5548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BD6317-8635-419A-A3FB-A0ED3DB5123B}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1527,7 +5762,7 @@
         <v>2.5439272640316669E-6</v>
       </c>
       <c r="I6" s="42">
-        <f t="shared" ref="I6:I8" si="0">H6/H$10</f>
+        <f t="shared" ref="I6" si="0">H6/H$10</f>
         <v>1.7720997321244589E-2</v>
       </c>
       <c r="J6" s="37">
@@ -1749,7 +5984,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:14" ht="82.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" ht="83" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="12"/>
       <c r="B16" s="14" t="s">
         <v>7</v>
@@ -2095,4 +6330,256 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8341A969-9B58-4390-812C-03CB54D5AEC6}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>25.6</v>
+      </c>
+      <c r="C2">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>4.7</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>26.8</v>
+      </c>
+      <c r="C5">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>1.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3DF5C8-00D1-42A3-BBE5-D82B9BAF2100}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>2.6</v>
+      </c>
+      <c r="C2">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1.8</v>
+      </c>
+      <c r="C4">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>5.9</v>
+      </c>
+      <c r="C5">
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>4.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB932818-3CDF-47AE-8148-B985FF30137D}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1.7</v>
+      </c>
+      <c r="C4">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>6.3</v>
+      </c>
+      <c r="C5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>